<commit_message>
Added rough ability to read simulator configuration from dataframe passed to simulator.
Still need to clean up code, but tired and will do in morning.  Code is functional though.
</commit_message>
<xml_diff>
--- a/neural_network_dev/simulator/0_benrules-realtime/mars_sim_config.xlsx
+++ b/neural_network_dev/simulator/0_benrules-realtime/mars_sim_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\0_demo-sim\benrules-realtime-simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\neural_network_dev\simulator\0_benrules-realtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13031DBB-2F95-4B77-A6F5-3595056D5973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E4CE3F-F2BA-4354-92F7-1B95B036F8B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8172" yWindow="1632" windowWidth="17280" windowHeight="8964" xr2:uid="{68A2E085-D47E-4EE5-818C-BE1060847917}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68A2E085-D47E-4EE5-818C-BE1060847917}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>